<commit_message>
Patched EXDC2 for default saturation parameters; added a test case for PMU.
</commit_message>
<xml_diff>
--- a/andes/cases/kundur/kundur_freq.xlsx
+++ b/andes/cases/kundur/kundur_freq.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcui7/repos/andes/andes/cases/kundur/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57388D7-AC73-D341-8E1A-6063A3F75FAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62ACF65C-0222-5048-B257-CEBDABFE187A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22240" yWindow="9540" windowWidth="29500" windowHeight="17460" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1322,7 +1322,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q5" sqref="Q5:T5"/>
+      <selection pane="bottomLeft" activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1445,10 +1445,10 @@
         <v>0</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
@@ -1507,10 +1507,10 @@
         <v>0</v>
       </c>
       <c r="S3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
@@ -1569,10 +1569,10 @@
         <v>0</v>
       </c>
       <c r="S4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
@@ -1631,10 +1631,10 @@
         <v>0</v>
       </c>
       <c r="S5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>